<commit_message>
Update Base.xlsx with latest data
</commit_message>
<xml_diff>
--- a/public/sample_data/Base.xlsx
+++ b/public/sample_data/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Machine Resale rate Caluclations\Machine Resale rate Caluclations\frontend\public\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/udaykirankodaru/Documents/Machine Resale rate Caluclations/frontend/public/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC2725-673D-42F6-9B6D-E769A381BEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E687ED-064D-7940-9792-A5FBB96A7845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="21800" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -834,17 +834,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="14.1875" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -895,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -912,7 +912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -929,9 +929,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -961,9 +961,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -977,7 +977,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1126,9 +1126,9 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>3507.65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>4231.6499999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>4505.6499999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>3863.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>3448.65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>4807.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>5930.081776654366</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>7035.4298306354358</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>8938.3041454286413</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>3372.65</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>3602.65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>3876.65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>3234.65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>2819.65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>4046.7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>5173.081776654366</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>6098.4298306354358</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -1519,9 +1519,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1576,9 +1576,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -1624,15 +1624,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5" customWidth="1"/>
-    <col min="3" max="3" width="34.1875" customWidth="1"/>
-    <col min="5" max="5" width="14.1875" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1763,13 +1763,17 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1815,7 +1819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1884,7 +1888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1944,35 +1948,35 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.6875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.6875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.6875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.6875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.6875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>0.42790590890399788</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>0.40623958624752182</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2394,7 +2398,7 @@
         <v>0.41896425193465858</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>0.34296016769527382</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2604,7 +2608,7 @@
         <v>0.42635831442853528</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>0.42035731616420707</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>0.37482466089648592</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2917,7 @@
         <v>0.54628209099542835</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>0.4925225661662479</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -3126,12 +3130,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3178,7 +3182,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3221,7 +3225,7 @@
         <v>147606.01216000001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3262,7 +3266,7 @@
         <v>108320.9376</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3303,7 +3307,7 @@
         <v>16690.024959999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>71401.070080000005</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3396,12 +3400,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -3448,7 +3452,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3486,7 +3490,7 @@
         <v>8703.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3524,7 +3528,7 @@
         <v>745.98</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3562,7 +3566,7 @@
         <v>14049.29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -3600,7 +3604,7 @@
         <v>4351.55</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3638,7 +3642,7 @@
         <v>41339.724999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3676,7 +3680,7 @@
         <v>37361.165000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -3727,12 +3731,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.3125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -3752,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>112</v>
       </c>
@@ -3764,7 +3768,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>113</v>
       </c>
@@ -3776,7 +3780,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>114</v>
       </c>
@@ -3788,7 +3792,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>115</v>
       </c>
@@ -3802,7 +3806,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>116</v>
       </c>
@@ -3814,7 +3818,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>117</v>
       </c>
@@ -3828,7 +3832,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>118</v>
       </c>
@@ -3866,12 +3870,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -3879,7 +3883,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -3887,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3895,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3903,7 +3907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -3911,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -3919,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3927,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -3949,15 +3953,15 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="23.6875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6875" customWidth="1"/>
-    <col min="5" max="5" width="41.1875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -3974,7 +3978,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -3991,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -4008,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4025,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4042,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -4059,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4076,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Add latest Base.xlsx for Render deploy (public/sample_data/Base.xlsx)
</commit_message>
<xml_diff>
--- a/public/sample_data/Base.xlsx
+++ b/public/sample_data/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/udaykirankodaru/Documents/Machine Resale rate Caluclations/frontend/public/sample_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Machine Resale rate Caluclations\Machine Resale rate Caluclations\frontend\public\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E687ED-064D-7940-9792-A5FBB96A7845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E337D0-D219-4E6A-BD92-143DF76751C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="21800" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <sheet name="QTC Parts" sheetId="6" r:id="rId6"/>
     <sheet name="Conversion matrix " sheetId="13" r:id="rId7"/>
     <sheet name="CoreQInventory" sheetId="7" r:id="rId8"/>
-    <sheet name="OutBase" sheetId="8" r:id="rId9"/>
-    <sheet name="OutProfit" sheetId="9" r:id="rId10"/>
-    <sheet name="ModelTable" sheetId="10" r:id="rId11"/>
-    <sheet name="Out_BB" sheetId="11" r:id="rId12"/>
-    <sheet name="Out_TOT" sheetId="12" r:id="rId13"/>
+    <sheet name="Scrap" sheetId="14" r:id="rId9"/>
+    <sheet name="OutBase" sheetId="8" r:id="rId10"/>
+    <sheet name="OutProfit" sheetId="9" r:id="rId11"/>
+    <sheet name="ModelTable" sheetId="10" r:id="rId12"/>
+    <sheet name="Out_BB" sheetId="11" r:id="rId13"/>
+    <sheet name="Out_TOT" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
   <si>
     <t xml:space="preserve"> System</t>
   </si>
@@ -74,9 +75,6 @@
     <t>850F</t>
   </si>
   <si>
-    <t>1150F</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -405,13 +403,40 @@
   </si>
   <si>
     <t>Wafer Stage (WS)</t>
+  </si>
+  <si>
+    <t>id_component</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>residual_value</t>
+  </si>
+  <si>
+    <t>scrap_value</t>
+  </si>
+  <si>
+    <t>PAS5500/100A</t>
+  </si>
+  <si>
+    <t>PAS5500/200</t>
+  </si>
+  <si>
+    <t>PAS5500/250C</t>
+  </si>
+  <si>
+    <t>PAS5500/3x0</t>
+  </si>
+  <si>
+    <t>PAS5500/22/60/80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -425,6 +450,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -487,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -497,6 +528,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,17 +871,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -878,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -895,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -912,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -929,9 +966,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -953,162 +990,326 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6875" customWidth="1"/>
+    <col min="5" max="5" width="41.1875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="6">
+        <v>350</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1200</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1400</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1200</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="6">
+        <v>725</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="D2">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
         <v>86</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
         <v>90</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7">
-        <v>7410</v>
-      </c>
-      <c r="D7">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8">
-        <v>825</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9">
-        <v>213</v>
-      </c>
-      <c r="D9">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" t="s">
-        <v>93</v>
-      </c>
       <c r="C11" s="7">
-        <v>8448</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1117,43 +1318,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
         <v>95</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>100</v>
-      </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1168,12 +1369,12 @@
         <v>3507.65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1188,12 +1389,12 @@
         <v>4231.6499999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1208,12 +1409,12 @@
         <v>4505.6499999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1228,12 +1429,12 @@
         <v>3863.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1248,12 +1449,12 @@
         <v>3448.65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1268,12 +1469,12 @@
         <v>4807.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1288,12 +1489,12 @@
         <v>5930.081776654366</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1308,15 +1509,15 @@
         <v>7035.4298306354358</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>13239.15</v>
@@ -1328,12 +1529,12 @@
         <v>8938.3041454286413</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1348,12 +1549,12 @@
         <v>3372.65</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1368,12 +1569,12 @@
         <v>3602.65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1388,12 +1589,12 @@
         <v>3876.65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1408,12 +1609,12 @@
         <v>3234.65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1428,12 +1629,12 @@
         <v>2819.65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1448,12 +1649,12 @@
         <v>4046.7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1468,12 +1669,12 @@
         <v>5173.081776654366</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1488,15 +1689,15 @@
         <v>6098.4298306354358</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>13239.15</v>
@@ -1513,28 +1714,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>104</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1543,9 +1744,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1554,9 +1755,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1570,41 +1771,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>108</v>
       </c>
       <c r="B2">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>30000</v>
@@ -1624,20 +1825,20 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1875" customWidth="1"/>
+    <col min="5" max="5" width="14.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1652,12 +1853,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1672,12 +1873,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1692,12 +1893,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1712,12 +1913,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1732,12 +1933,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1767,21 +1968,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1796,15 +1993,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>5</v>
@@ -1819,15 +2016,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2">
         <v>6</v>
@@ -1842,15 +2039,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
@@ -1865,15 +2062,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>7</v>
@@ -1888,15 +2085,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -1911,15 +2108,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -1945,150 +2142,150 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="11.6875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6875" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.6875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6875" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6">
         <v>350</v>
@@ -2188,12 +2385,12 @@
         <v>0.42790590890399788</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="6">
         <v>1200</v>
@@ -2293,12 +2490,12 @@
         <v>0.40623958624752182</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6">
         <v>1400</v>
@@ -2398,12 +2595,12 @@
         <v>0.41896425193465858</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="6">
         <v>1200</v>
@@ -2503,12 +2700,12 @@
         <v>0.34296016769527382</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="6">
         <v>300</v>
@@ -2608,12 +2805,12 @@
         <v>0.42635831442853528</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6">
         <v>1200</v>
@@ -2713,12 +2910,12 @@
         <v>0.42035731616420707</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="6">
         <v>300</v>
@@ -2818,12 +3015,12 @@
         <v>0.37482466089648592</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="6">
         <v>725</v>
@@ -2917,12 +3114,12 @@
         <v>0.54628209099542835</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="6">
         <v>725</v>
@@ -3016,12 +3213,12 @@
         <v>0.4925225661662479</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="6">
         <v>1000</v>
@@ -3130,61 +3327,61 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6">
         <v>131000</v>
@@ -3225,9 +3422,9 @@
         <v>147606.01216000001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6">
@@ -3266,9 +3463,9 @@
         <v>108320.9376</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -3307,9 +3504,9 @@
         <v>16690.024959999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6">
@@ -3348,9 +3545,9 @@
         <v>71401.070080000005</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -3400,61 +3597,61 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>14000</v>
@@ -3490,9 +3687,9 @@
         <v>8703.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>1200</v>
@@ -3528,9 +3725,9 @@
         <v>745.98</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>22600</v>
@@ -3566,9 +3763,9 @@
         <v>14049.29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>7000</v>
@@ -3604,9 +3801,9 @@
         <v>4351.55</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>66500</v>
@@ -3642,9 +3839,9 @@
         <v>41339.724999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>60100</v>
@@ -3680,9 +3877,9 @@
         <v>37361.165000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>6300</v>
@@ -3728,17 +3925,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>5</v>
@@ -3753,95 +3950,97 @@
         <v>8</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1">
-        <v>3022.6499999999996</v>
+        <v>2620.4700000000003</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1">
-        <v>2402.6499999999996</v>
+        <v>3344.4769499999993</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="8">
-        <v>2476.6499999999996</v>
+        <v>3618.4769499999993</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="8">
-        <v>2034.6499999999996</v>
+        <v>2976.4769499999993</v>
       </c>
       <c r="C5" s="8">
-        <v>2846.7</v>
+        <v>3788.5269499999986</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="8">
-        <v>2519.6499999999996</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>2561.4769499999993</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2584.5269499999986</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8">
-        <v>4448.081776654366</v>
+        <v>4914.9087266543665</v>
       </c>
       <c r="E7" s="8">
-        <v>5373.4298306354358</v>
+        <v>5783.5303306354363</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8">
-        <v>7001.3041454286413</v>
+        <v>7686.4046454286417</v>
       </c>
     </row>
   </sheetData>
@@ -3866,74 +4065,74 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>112</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>113</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>114</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>116</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>117</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>118</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3945,156 +4144,296 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAECB185-8425-4F7A-9340-7AA72BCD849E}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
         <v>118</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Push latest base file
</commit_message>
<xml_diff>
--- a/public/sample_data/Base.xlsx
+++ b/public/sample_data/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Machine Resale rate Caluclations\Machine Resale rate Caluclations\frontend\public\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/udaykirankodaru/Documents/Machine Resale rate Caluclations/public/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E337D0-D219-4E6A-BD92-143DF76751C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A48627-FB41-F14A-9A19-6EF52DFE1EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="130">
   <si>
     <t xml:space="preserve"> System</t>
   </si>
@@ -324,9 +324,6 @@
     <t>mnull</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Profit</t>
   </si>
   <si>
@@ -430,6 +427,15 @@
   </si>
   <si>
     <t>PAS5500/22/60/80</t>
+  </si>
+  <si>
+    <t>Total Without Scrap</t>
+  </si>
+  <si>
+    <t>Scrap</t>
+  </si>
+  <si>
+    <t>Total With Scrap</t>
   </si>
 </sst>
 </file>
@@ -875,13 +881,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="14.1875" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -915,7 +921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -932,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -949,7 +955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -966,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -998,15 +1004,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="23.6875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6875" customWidth="1"/>
-    <col min="5" max="5" width="41.1875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1023,9 +1029,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="6">
         <v>350</v>
@@ -1040,9 +1046,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="6">
         <v>1200</v>
@@ -1057,9 +1063,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="6">
         <v>1400</v>
@@ -1074,9 +1080,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="6">
         <v>1200</v>
@@ -1091,9 +1097,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="6">
         <v>300</v>
@@ -1108,9 +1114,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="6">
         <v>725</v>
@@ -1125,9 +1131,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="6">
         <v>1000</v>
@@ -1150,15 +1156,15 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1172,7 +1178,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1228,12 +1234,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>87</v>
@@ -1242,73 +1248,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
         <v>86</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
         <v>89</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
         <v>90</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>0</v>
       </c>
     </row>
@@ -1327,34 +1389,34 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>81</v>
       </c>
       <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1369,12 +1431,12 @@
         <v>3507.65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1389,12 +1451,12 @@
         <v>4231.6499999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1409,12 +1471,12 @@
         <v>4505.6499999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1429,12 +1491,12 @@
         <v>3863.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1449,12 +1511,12 @@
         <v>3448.65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1469,12 +1531,12 @@
         <v>4807.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1489,12 +1551,12 @@
         <v>5930.081776654366</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1509,12 +1571,12 @@
         <v>7035.4298306354358</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
@@ -1529,12 +1591,12 @@
         <v>8938.3041454286413</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1549,12 +1611,12 @@
         <v>3372.65</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1569,12 +1631,12 @@
         <v>3602.65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1589,12 +1651,12 @@
         <v>3876.65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1609,12 +1671,12 @@
         <v>3234.65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1629,12 +1691,12 @@
         <v>2819.65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1649,12 +1711,12 @@
         <v>4046.7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1669,12 +1731,12 @@
         <v>5173.081776654366</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1689,12 +1751,12 @@
         <v>6098.4298306354358</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
@@ -1720,22 +1782,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>103</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1744,9 +1806,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1755,9 +1817,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1777,35 +1839,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
       <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>107</v>
       </c>
       <c r="B2">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>30000</v>
@@ -1825,15 +1887,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5" customWidth="1"/>
-    <col min="3" max="3" width="34.1875" customWidth="1"/>
-    <col min="5" max="5" width="14.1875" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1853,7 +1915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1873,9 +1935,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -1893,7 +1955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1913,7 +1975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1933,7 +1995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1968,9 +2030,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1993,7 +2055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -2039,7 +2101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2062,7 +2124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2085,7 +2147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2108,7 +2170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2141,39 +2203,39 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.6875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.6875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.6875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.6875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.6875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2280,12 +2342,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="6">
         <v>350</v>
@@ -2385,12 +2447,12 @@
         <v>0.42790590890399788</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6">
         <v>1200</v>
@@ -2490,12 +2552,12 @@
         <v>0.40623958624752182</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="6">
         <v>1400</v>
@@ -2595,12 +2657,12 @@
         <v>0.41896425193465858</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="6">
         <v>1200</v>
@@ -2700,12 +2762,12 @@
         <v>0.34296016769527382</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="6">
         <v>300</v>
@@ -2805,12 +2867,12 @@
         <v>0.42635831442853528</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="6">
         <v>1200</v>
@@ -2910,12 +2972,12 @@
         <v>0.42035731616420707</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="6">
         <v>300</v>
@@ -3015,12 +3077,12 @@
         <v>0.37482466089648592</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="6">
         <v>725</v>
@@ -3114,12 +3176,12 @@
         <v>0.54628209099542835</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="6">
         <v>725</v>
@@ -3213,12 +3275,12 @@
         <v>0.4925225661662479</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="6">
         <v>1000</v>
@@ -3327,12 +3389,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -3379,7 +3441,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3422,9 +3484,9 @@
         <v>147606.01216000001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6">
@@ -3463,7 +3525,7 @@
         <v>108320.9376</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3504,7 +3566,7 @@
         <v>16690.024959999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3545,7 +3607,7 @@
         <v>71401.070080000005</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3597,12 +3659,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -3649,7 +3711,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3687,7 +3749,7 @@
         <v>8703.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3725,7 +3787,7 @@
         <v>745.98</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3763,7 +3825,7 @@
         <v>14049.29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3801,7 +3863,7 @@
         <v>4351.55</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3839,7 +3901,7 @@
         <v>41339.724999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3877,7 +3939,7 @@
         <v>37361.165000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -3928,14 +3990,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.3125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>5</v>
@@ -3953,9 +4015,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1">
         <v>2620.4700000000003</v>
@@ -3965,9 +4027,9 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1">
         <v>3344.4769499999993</v>
@@ -3977,9 +4039,9 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="8">
         <v>3618.4769499999993</v>
@@ -3989,9 +4051,9 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="8">
         <v>2976.4769499999993</v>
@@ -4003,9 +4065,9 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="8">
         <v>2561.4769499999993</v>
@@ -4017,9 +4079,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -4031,9 +4093,9 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -4065,16 +4127,16 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4082,57 +4144,57 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>111</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>112</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>113</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>114</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>115</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>116</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>117</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4151,28 +4213,28 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>123</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>10</v>
@@ -4184,9 +4246,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>10</v>
@@ -4198,9 +4260,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
@@ -4212,9 +4274,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -4226,9 +4288,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
@@ -4240,9 +4302,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
@@ -4254,9 +4316,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>10</v>
@@ -4268,7 +4330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -4282,9 +4344,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>9</v>
@@ -4296,7 +4358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4310,7 +4372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4324,7 +4386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -4338,7 +4400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -4352,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4366,7 +4428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4380,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -4394,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4408,7 +4470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4422,7 +4484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>

</xml_diff>